<commit_message>
Mean, Median Standart Dev. etc. + New Files Added and Small Improvements
</commit_message>
<xml_diff>
--- a/Assignment_2/temizlenmiş_veri_0.xlsx
+++ b/Assignment_2/temizlenmiş_veri_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B573"/>
+  <dimension ref="A1:A573"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,4588 +436,2867 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
           <t>Fiyat</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>36</v>
-      </c>
-      <c r="B2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>133</v>
-      </c>
-      <c r="B3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>153</v>
-      </c>
-      <c r="B4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>431</v>
-      </c>
-      <c r="B5" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>293</v>
-      </c>
-      <c r="B6" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>101</v>
-      </c>
-      <c r="B7" t="n">
         <v>350</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>447</v>
-      </c>
-      <c r="B8" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>473</v>
-      </c>
-      <c r="B9" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>91</v>
-      </c>
-      <c r="B10" t="n">
         <v>400</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>213</v>
-      </c>
-      <c r="B11" t="n">
         <v>5000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>179</v>
-      </c>
-      <c r="B12" t="n">
         <v>7500</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>467</v>
-      </c>
-      <c r="B13" t="n">
         <v>9000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>330</v>
-      </c>
-      <c r="B14" t="n">
         <v>9300</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>228</v>
-      </c>
-      <c r="B15" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>494</v>
-      </c>
-      <c r="B16" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>506</v>
-      </c>
-      <c r="B17" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>231</v>
-      </c>
-      <c r="B18" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>21</v>
-      </c>
-      <c r="B19" t="n">
         <v>10500</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>86</v>
-      </c>
-      <c r="B20" t="n">
         <v>10500</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>403</v>
-      </c>
-      <c r="B21" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>465</v>
-      </c>
-      <c r="B22" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>501</v>
-      </c>
-      <c r="B23" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>59</v>
-      </c>
-      <c r="B24" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>434</v>
-      </c>
-      <c r="B25" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>51</v>
-      </c>
-      <c r="B26" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>40</v>
-      </c>
-      <c r="B27" t="n">
         <v>11000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>511</v>
-      </c>
-      <c r="B28" t="n">
         <v>11250</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>340</v>
-      </c>
-      <c r="B29" t="n">
         <v>11500</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>556</v>
-      </c>
-      <c r="B30" t="n">
         <v>11500</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>121</v>
-      </c>
-      <c r="B31" t="n">
         <v>11500</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>569</v>
-      </c>
-      <c r="B33" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>92</v>
-      </c>
-      <c r="B34" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>564</v>
-      </c>
-      <c r="B35" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>201</v>
-      </c>
-      <c r="B36" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>214</v>
-      </c>
-      <c r="B37" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>355</v>
-      </c>
-      <c r="B38" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>348</v>
-      </c>
-      <c r="B39" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>383</v>
-      </c>
-      <c r="B40" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>116</v>
-      </c>
-      <c r="B41" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>14</v>
-      </c>
-      <c r="B42" t="n">
         <v>12000</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>498</v>
-      </c>
-      <c r="B43" t="n">
         <v>12450</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>497</v>
-      </c>
-      <c r="B44" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>409</v>
-      </c>
-      <c r="B45" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>263</v>
-      </c>
-      <c r="B46" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>268</v>
-      </c>
-      <c r="B47" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>386</v>
-      </c>
-      <c r="B48" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9</v>
-      </c>
-      <c r="B49" t="n">
         <v>12500</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>145</v>
-      </c>
-      <c r="B50" t="n">
         <v>12750</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>535</v>
-      </c>
-      <c r="B51" t="n">
         <v>12999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>311</v>
-      </c>
-      <c r="B52" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>345</v>
-      </c>
-      <c r="B53" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>65</v>
-      </c>
-      <c r="B54" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>520</v>
-      </c>
-      <c r="B55" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>421</v>
-      </c>
-      <c r="B56" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>185</v>
-      </c>
-      <c r="B57" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5</v>
-      </c>
-      <c r="B58" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>130</v>
-      </c>
-      <c r="B59" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>419</v>
-      </c>
-      <c r="B60" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>83</v>
-      </c>
-      <c r="B61" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2</v>
-      </c>
-      <c r="B62" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>464</v>
-      </c>
-      <c r="B63" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>544</v>
-      </c>
-      <c r="B64" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>33</v>
-      </c>
-      <c r="B65" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>550</v>
-      </c>
-      <c r="B66" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>239</v>
-      </c>
-      <c r="B67" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>202</v>
-      </c>
-      <c r="B68" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>160</v>
-      </c>
-      <c r="B69" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>290</v>
-      </c>
-      <c r="B70" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>267</v>
-      </c>
-      <c r="B71" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>226</v>
-      </c>
-      <c r="B72" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>289</v>
-      </c>
-      <c r="B73" t="n">
         <v>13000</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>426</v>
-      </c>
-      <c r="B74" t="n">
         <v>13250</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>102</v>
-      </c>
-      <c r="B75" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>245</v>
-      </c>
-      <c r="B76" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>204</v>
-      </c>
-      <c r="B77" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>227</v>
-      </c>
-      <c r="B78" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>114</v>
-      </c>
-      <c r="B79" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>138</v>
-      </c>
-      <c r="B80" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>38</v>
-      </c>
-      <c r="B81" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>525</v>
-      </c>
-      <c r="B82" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>326</v>
-      </c>
-      <c r="B83" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>396</v>
-      </c>
-      <c r="B84" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>487</v>
-      </c>
-      <c r="B85" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>536</v>
-      </c>
-      <c r="B86" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>529</v>
-      </c>
-      <c r="B87" t="n">
         <v>13500</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>475</v>
-      </c>
-      <c r="B88" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>332</v>
-      </c>
-      <c r="B89" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>408</v>
-      </c>
-      <c r="B90" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>527</v>
-      </c>
-      <c r="B91" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>537</v>
-      </c>
-      <c r="B92" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>546</v>
-      </c>
-      <c r="B93" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>461</v>
-      </c>
-      <c r="B94" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>486</v>
-      </c>
-      <c r="B95" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>389</v>
-      </c>
-      <c r="B96" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>369</v>
-      </c>
-      <c r="B97" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>171</v>
-      </c>
-      <c r="B98" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>555</v>
-      </c>
-      <c r="B99" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>243</v>
-      </c>
-      <c r="B100" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>106</v>
-      </c>
-      <c r="B101" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>378</v>
-      </c>
-      <c r="B102" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>432</v>
-      </c>
-      <c r="B103" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>387</v>
-      </c>
-      <c r="B104" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>260</v>
-      </c>
-      <c r="B105" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>557</v>
-      </c>
-      <c r="B106" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>147</v>
-      </c>
-      <c r="B107" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>257</v>
-      </c>
-      <c r="B108" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>137</v>
-      </c>
-      <c r="B109" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>250</v>
-      </c>
-      <c r="B110" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>94</v>
-      </c>
-      <c r="B111" t="n">
         <v>14000</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>0</v>
-      </c>
-      <c r="B112" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>513</v>
-      </c>
-      <c r="B113" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>347</v>
-      </c>
-      <c r="B114" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>466</v>
-      </c>
-      <c r="B115" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>200</v>
-      </c>
-      <c r="B116" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>262</v>
-      </c>
-      <c r="B117" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>132</v>
-      </c>
-      <c r="B118" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>16</v>
-      </c>
-      <c r="B119" t="n">
         <v>14500</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>542</v>
-      </c>
-      <c r="B120" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>543</v>
-      </c>
-      <c r="B121" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>67</v>
-      </c>
-      <c r="B122" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>159</v>
-      </c>
-      <c r="B123" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>177</v>
-      </c>
-      <c r="B124" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>424</v>
-      </c>
-      <c r="B125" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>406</v>
-      </c>
-      <c r="B126" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>64</v>
-      </c>
-      <c r="B127" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>143</v>
-      </c>
-      <c r="B128" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>140</v>
-      </c>
-      <c r="B129" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>136</v>
-      </c>
-      <c r="B130" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>193</v>
-      </c>
-      <c r="B131" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>548</v>
-      </c>
-      <c r="B132" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>173</v>
-      </c>
-      <c r="B133" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>167</v>
-      </c>
-      <c r="B134" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>134</v>
-      </c>
-      <c r="B135" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>166</v>
-      </c>
-      <c r="B136" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>164</v>
-      </c>
-      <c r="B137" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>519</v>
-      </c>
-      <c r="B138" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>401</v>
-      </c>
-      <c r="B139" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>412</v>
-      </c>
-      <c r="B140" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>402</v>
-      </c>
-      <c r="B141" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>181</v>
-      </c>
-      <c r="B142" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>502</v>
-      </c>
-      <c r="B143" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>192</v>
-      </c>
-      <c r="B144" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>235</v>
-      </c>
-      <c r="B145" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>234</v>
-      </c>
-      <c r="B146" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>218</v>
-      </c>
-      <c r="B147" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>107</v>
-      </c>
-      <c r="B148" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>222</v>
-      </c>
-      <c r="B149" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>115</v>
-      </c>
-      <c r="B150" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>203</v>
-      </c>
-      <c r="B151" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>492</v>
-      </c>
-      <c r="B152" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>490</v>
-      </c>
-      <c r="B153" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>489</v>
-      </c>
-      <c r="B154" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>484</v>
-      </c>
-      <c r="B155" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>255</v>
-      </c>
-      <c r="B156" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>229</v>
-      </c>
-      <c r="B157" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>249</v>
-      </c>
-      <c r="B158" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>384</v>
-      </c>
-      <c r="B159" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>215</v>
-      </c>
-      <c r="B160" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>53</v>
-      </c>
-      <c r="B161" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>458</v>
-      </c>
-      <c r="B162" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>56</v>
-      </c>
-      <c r="B163" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>97</v>
-      </c>
-      <c r="B164" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>247</v>
-      </c>
-      <c r="B165" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>55</v>
-      </c>
-      <c r="B166" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>251</v>
-      </c>
-      <c r="B167" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>296</v>
-      </c>
-      <c r="B168" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>454</v>
-      </c>
-      <c r="B169" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>308</v>
-      </c>
-      <c r="B170" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>309</v>
-      </c>
-      <c r="B171" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>478</v>
-      </c>
-      <c r="B172" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>476</v>
-      </c>
-      <c r="B173" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>441</v>
-      </c>
-      <c r="B174" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>81</v>
-      </c>
-      <c r="B175" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>50</v>
-      </c>
-      <c r="B176" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>436</v>
-      </c>
-      <c r="B177" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>283</v>
-      </c>
-      <c r="B178" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>284</v>
-      </c>
-      <c r="B179" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>286</v>
-      </c>
-      <c r="B180" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>271</v>
-      </c>
-      <c r="B181" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>269</v>
-      </c>
-      <c r="B182" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>84</v>
-      </c>
-      <c r="B183" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>568</v>
-      </c>
-      <c r="B184" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>32</v>
-      </c>
-      <c r="B185" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>34</v>
-      </c>
-      <c r="B186" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>27</v>
-      </c>
-      <c r="B187" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>162</v>
-      </c>
-      <c r="B188" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>480</v>
-      </c>
-      <c r="B189" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>291</v>
-      </c>
-      <c r="B190" t="n">
         <v>15250</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>462</v>
-      </c>
-      <c r="B191" t="n">
         <v>15300</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>44</v>
-      </c>
-      <c r="B192" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>398</v>
-      </c>
-      <c r="B193" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>549</v>
-      </c>
-      <c r="B194" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>353</v>
-      </c>
-      <c r="B195" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>363</v>
-      </c>
-      <c r="B196" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>28</v>
-      </c>
-      <c r="B197" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>127</v>
-      </c>
-      <c r="B198" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>302</v>
-      </c>
-      <c r="B199" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>376</v>
-      </c>
-      <c r="B200" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>210</v>
-      </c>
-      <c r="B201" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>198</v>
-      </c>
-      <c r="B202" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>232</v>
-      </c>
-      <c r="B203" t="n">
         <v>15500</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>125</v>
-      </c>
-      <c r="B204" t="n">
         <v>15750</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>451</v>
-      </c>
-      <c r="B205" t="n">
         <v>15750</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>230</v>
-      </c>
-      <c r="B206" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>474</v>
-      </c>
-      <c r="B207" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>566</v>
-      </c>
-      <c r="B208" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>117</v>
-      </c>
-      <c r="B209" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>123</v>
-      </c>
-      <c r="B210" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>35</v>
-      </c>
-      <c r="B211" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>85</v>
-      </c>
-      <c r="B212" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>266</v>
-      </c>
-      <c r="B213" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>306</v>
-      </c>
-      <c r="B214" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>367</v>
-      </c>
-      <c r="B215" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>328</v>
-      </c>
-      <c r="B216" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>259</v>
-      </c>
-      <c r="B217" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>456</v>
-      </c>
-      <c r="B218" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>488</v>
-      </c>
-      <c r="B219" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>158</v>
-      </c>
-      <c r="B220" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>63</v>
-      </c>
-      <c r="B221" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>563</v>
-      </c>
-      <c r="B222" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>435</v>
-      </c>
-      <c r="B223" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>517</v>
-      </c>
-      <c r="B224" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>460</v>
-      </c>
-      <c r="B225" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>52</v>
-      </c>
-      <c r="B226" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>559</v>
-      </c>
-      <c r="B227" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>540</v>
-      </c>
-      <c r="B228" t="n">
         <v>16000</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>142</v>
-      </c>
-      <c r="B229" t="n">
         <v>16250</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>221</v>
-      </c>
-      <c r="B230" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>72</v>
-      </c>
-      <c r="B231" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>148</v>
-      </c>
-      <c r="B232" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>407</v>
-      </c>
-      <c r="B233" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>485</v>
-      </c>
-      <c r="B234" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>341</v>
-      </c>
-      <c r="B235" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>8</v>
-      </c>
-      <c r="B236" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>13</v>
-      </c>
-      <c r="B237" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>119</v>
-      </c>
-      <c r="B238" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>241</v>
-      </c>
-      <c r="B239" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>404</v>
-      </c>
-      <c r="B240" t="n">
         <v>16500</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>318</v>
-      </c>
-      <c r="B241" t="n">
         <v>16950</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>414</v>
-      </c>
-      <c r="B242" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>413</v>
-      </c>
-      <c r="B243" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>457</v>
-      </c>
-      <c r="B244" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>512</v>
-      </c>
-      <c r="B245" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>73</v>
-      </c>
-      <c r="B246" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>515</v>
-      </c>
-      <c r="B247" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>122</v>
-      </c>
-      <c r="B248" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>479</v>
-      </c>
-      <c r="B249" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>351</v>
-      </c>
-      <c r="B250" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>481</v>
-      </c>
-      <c r="B251" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>360</v>
-      </c>
-      <c r="B252" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>483</v>
-      </c>
-      <c r="B253" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>385</v>
-      </c>
-      <c r="B254" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>69</v>
-      </c>
-      <c r="B255" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>191</v>
-      </c>
-      <c r="B256" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>405</v>
-      </c>
-      <c r="B257" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>135</v>
-      </c>
-      <c r="B258" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>74</v>
-      </c>
-      <c r="B259" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>220</v>
-      </c>
-      <c r="B260" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>129</v>
-      </c>
-      <c r="B261" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>371</v>
-      </c>
-      <c r="B262" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>20</v>
-      </c>
-      <c r="B263" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>298</v>
-      </c>
-      <c r="B264" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>304</v>
-      </c>
-      <c r="B265" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>273</v>
-      </c>
-      <c r="B266" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>277</v>
-      </c>
-      <c r="B267" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>496</v>
-      </c>
-      <c r="B268" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>11</v>
-      </c>
-      <c r="B269" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>453</v>
-      </c>
-      <c r="B270" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>45</v>
-      </c>
-      <c r="B271" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>26</v>
-      </c>
-      <c r="B272" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>359</v>
-      </c>
-      <c r="B273" t="n">
         <v>17000</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>163</v>
-      </c>
-      <c r="B274" t="n">
         <v>17250</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>562</v>
-      </c>
-      <c r="B275" t="n">
         <v>17250</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>252</v>
-      </c>
-      <c r="B276" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>41</v>
-      </c>
-      <c r="B277" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>90</v>
-      </c>
-      <c r="B278" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>89</v>
-      </c>
-      <c r="B279" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>236</v>
-      </c>
-      <c r="B280" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>256</v>
-      </c>
-      <c r="B281" t="n">
         <v>17500</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>482</v>
-      </c>
-      <c r="B282" t="n">
         <v>17555</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>280</v>
-      </c>
-      <c r="B283" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>319</v>
-      </c>
-      <c r="B284" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>338</v>
-      </c>
-      <c r="B285" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>329</v>
-      </c>
-      <c r="B286" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>346</v>
-      </c>
-      <c r="B287" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>495</v>
-      </c>
-      <c r="B288" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>209</v>
-      </c>
-      <c r="B289" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>100</v>
-      </c>
-      <c r="B290" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>510</v>
-      </c>
-      <c r="B291" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>449</v>
-      </c>
-      <c r="B292" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>450</v>
-      </c>
-      <c r="B293" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>109</v>
-      </c>
-      <c r="B294" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>105</v>
-      </c>
-      <c r="B295" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>518</v>
-      </c>
-      <c r="B296" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>139</v>
-      </c>
-      <c r="B297" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>561</v>
-      </c>
-      <c r="B298" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>146</v>
-      </c>
-      <c r="B299" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>538</v>
-      </c>
-      <c r="B300" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>183</v>
-      </c>
-      <c r="B301" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>551</v>
-      </c>
-      <c r="B302" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>165</v>
-      </c>
-      <c r="B303" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>182</v>
-      </c>
-      <c r="B304" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>104</v>
-      </c>
-      <c r="B305" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>68</v>
-      </c>
-      <c r="B306" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>211</v>
-      </c>
-      <c r="B307" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>547</v>
-      </c>
-      <c r="B308" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>545</v>
-      </c>
-      <c r="B309" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>154</v>
-      </c>
-      <c r="B310" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>157</v>
-      </c>
-      <c r="B311" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>30</v>
-      </c>
-      <c r="B312" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>120</v>
-      </c>
-      <c r="B313" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>471</v>
-      </c>
-      <c r="B314" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>532</v>
-      </c>
-      <c r="B315" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>29</v>
-      </c>
-      <c r="B316" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>4</v>
-      </c>
-      <c r="B317" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>46</v>
-      </c>
-      <c r="B318" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>352</v>
-      </c>
-      <c r="B319" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>368</v>
-      </c>
-      <c r="B320" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>295</v>
-      </c>
-      <c r="B321" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>275</v>
-      </c>
-      <c r="B322" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>261</v>
-      </c>
-      <c r="B323" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>49</v>
-      </c>
-      <c r="B324" t="n">
         <v>18000</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>391</v>
-      </c>
-      <c r="B325" t="n">
         <v>18250</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>394</v>
-      </c>
-      <c r="B326" t="n">
         <v>18250</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>62</v>
-      </c>
-      <c r="B327" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>23</v>
-      </c>
-      <c r="B328" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>95</v>
-      </c>
-      <c r="B329" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>400</v>
-      </c>
-      <c r="B330" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>108</v>
-      </c>
-      <c r="B331" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>194</v>
-      </c>
-      <c r="B332" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>18</v>
-      </c>
-      <c r="B333" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>327</v>
-      </c>
-      <c r="B334" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>272</v>
-      </c>
-      <c r="B335" t="n">
         <v>18500</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>523</v>
-      </c>
-      <c r="B336" t="n">
         <v>18750</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>324</v>
-      </c>
-      <c r="B337" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>31</v>
-      </c>
-      <c r="B338" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>312</v>
-      </c>
-      <c r="B339" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>470</v>
-      </c>
-      <c r="B340" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>305</v>
-      </c>
-      <c r="B341" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>281</v>
-      </c>
-      <c r="B342" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>514</v>
-      </c>
-      <c r="B343" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>110</v>
-      </c>
-      <c r="B344" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>531</v>
-      </c>
-      <c r="B345" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>66</v>
-      </c>
-      <c r="B346" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>423</v>
-      </c>
-      <c r="B347" t="n">
         <v>19000</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>195</v>
-      </c>
-      <c r="B348" t="n">
         <v>19450</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>199</v>
-      </c>
-      <c r="B349" t="n">
         <v>19500</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>361</v>
-      </c>
-      <c r="B350" t="n">
         <v>19500</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>331</v>
-      </c>
-      <c r="B351" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>342</v>
-      </c>
-      <c r="B352" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>47</v>
-      </c>
-      <c r="B353" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>366</v>
-      </c>
-      <c r="B354" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>315</v>
-      </c>
-      <c r="B355" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>317</v>
-      </c>
-      <c r="B356" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>79</v>
-      </c>
-      <c r="B357" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>442</v>
-      </c>
-      <c r="B358" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>297</v>
-      </c>
-      <c r="B359" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>440</v>
-      </c>
-      <c r="B360" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>468</v>
-      </c>
-      <c r="B361" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>80</v>
-      </c>
-      <c r="B362" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>325</v>
-      </c>
-      <c r="B363" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>477</v>
-      </c>
-      <c r="B364" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>313</v>
-      </c>
-      <c r="B365" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>310</v>
-      </c>
-      <c r="B366" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>124</v>
-      </c>
-      <c r="B367" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>25</v>
-      </c>
-      <c r="B368" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>224</v>
-      </c>
-      <c r="B369" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>238</v>
-      </c>
-      <c r="B370" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>433</v>
-      </c>
-      <c r="B371" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>493</v>
-      </c>
-      <c r="B372" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>380</v>
-      </c>
-      <c r="B373" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>265</v>
-      </c>
-      <c r="B374" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>60</v>
-      </c>
-      <c r="B375" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>264</v>
-      </c>
-      <c r="B376" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>96</v>
-      </c>
-      <c r="B377" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>77</v>
-      </c>
-      <c r="B378" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>88</v>
-      </c>
-      <c r="B379" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>491</v>
-      </c>
-      <c r="B380" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>248</v>
-      </c>
-      <c r="B381" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>509</v>
-      </c>
-      <c r="B382" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>244</v>
-      </c>
-      <c r="B383" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>61</v>
-      </c>
-      <c r="B384" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>379</v>
-      </c>
-      <c r="B385" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>377</v>
-      </c>
-      <c r="B386" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>375</v>
-      </c>
-      <c r="B387" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>399</v>
-      </c>
-      <c r="B388" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>170</v>
-      </c>
-      <c r="B389" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>169</v>
-      </c>
-      <c r="B390" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>528</v>
-      </c>
-      <c r="B391" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>521</v>
-      </c>
-      <c r="B392" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>410</v>
-      </c>
-      <c r="B393" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>180</v>
-      </c>
-      <c r="B394" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>362</v>
-      </c>
-      <c r="B395" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>274</v>
-      </c>
-      <c r="B396" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>276</v>
-      </c>
-      <c r="B397" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>282</v>
-      </c>
-      <c r="B398" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>571</v>
-      </c>
-      <c r="B399" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>565</v>
-      </c>
-      <c r="B400" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>553</v>
-      </c>
-      <c r="B401" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>172</v>
-      </c>
-      <c r="B402" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>128</v>
-      </c>
-      <c r="B403" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>175</v>
-      </c>
-      <c r="B404" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>150</v>
-      </c>
-      <c r="B405" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>427</v>
-      </c>
-      <c r="B406" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>188</v>
-      </c>
-      <c r="B407" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>500</v>
-      </c>
-      <c r="B408" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>393</v>
-      </c>
-      <c r="B409" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>390</v>
-      </c>
-      <c r="B410" t="n">
         <v>20000</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="n">
-        <v>285</v>
-      </c>
-      <c r="B411" t="n">
         <v>20500</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>58</v>
-      </c>
-      <c r="B412" t="n">
         <v>20500</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="n">
-        <v>335</v>
-      </c>
-      <c r="B413" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>294</v>
-      </c>
-      <c r="B414" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>357</v>
-      </c>
-      <c r="B415" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>534</v>
-      </c>
-      <c r="B416" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="n">
-        <v>206</v>
-      </c>
-      <c r="B417" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>415</v>
-      </c>
-      <c r="B418" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="n">
-        <v>205</v>
-      </c>
-      <c r="B419" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>397</v>
-      </c>
-      <c r="B420" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
-        <v>187</v>
-      </c>
-      <c r="B421" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
-        <v>212</v>
-      </c>
-      <c r="B422" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
-        <v>448</v>
-      </c>
-      <c r="B423" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="n">
-        <v>54</v>
-      </c>
-      <c r="B424" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
-        <v>103</v>
-      </c>
-      <c r="B425" t="n">
         <v>21000</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
-        <v>508</v>
-      </c>
-      <c r="B426" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
-        <v>307</v>
-      </c>
-      <c r="B427" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
-        <v>459</v>
-      </c>
-      <c r="B428" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
-        <v>37</v>
-      </c>
-      <c r="B429" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
-        <v>258</v>
-      </c>
-      <c r="B430" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
-        <v>196</v>
-      </c>
-      <c r="B431" t="n">
         <v>21500</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
-        <v>12</v>
-      </c>
-      <c r="B432" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>144</v>
-      </c>
-      <c r="B433" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="n">
-        <v>7</v>
-      </c>
-      <c r="B434" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="n">
-        <v>560</v>
-      </c>
-      <c r="B435" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
-        <v>395</v>
-      </c>
-      <c r="B436" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
-        <v>446</v>
-      </c>
-      <c r="B437" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
-        <v>57</v>
-      </c>
-      <c r="B438" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
-        <v>437</v>
-      </c>
-      <c r="B439" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="n">
-        <v>279</v>
-      </c>
-      <c r="B440" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
-        <v>443</v>
-      </c>
-      <c r="B441" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="n">
-        <v>472</v>
-      </c>
-      <c r="B442" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="n">
-        <v>320</v>
-      </c>
-      <c r="B443" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="n">
-        <v>98</v>
-      </c>
-      <c r="B444" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="n">
-        <v>278</v>
-      </c>
-      <c r="B445" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="n">
-        <v>208</v>
-      </c>
-      <c r="B446" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="n">
-        <v>207</v>
-      </c>
-      <c r="B447" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
-        <v>428</v>
-      </c>
-      <c r="B448" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
-        <v>422</v>
-      </c>
-      <c r="B449" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
-        <v>526</v>
-      </c>
-      <c r="B450" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
-        <v>15</v>
-      </c>
-      <c r="B451" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
-        <v>151</v>
-      </c>
-      <c r="B452" t="n">
         <v>22000</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
-        <v>455</v>
-      </c>
-      <c r="B453" t="n">
         <v>22500</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="n">
-        <v>364</v>
-      </c>
-      <c r="B454" t="n">
         <v>22500</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="n">
-        <v>503</v>
-      </c>
-      <c r="B455" t="n">
         <v>22500</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
-        <v>152</v>
-      </c>
-      <c r="B456" t="n">
         <v>22500</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
-        <v>156</v>
-      </c>
-      <c r="B457" t="n">
         <v>22500</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
-        <v>22</v>
-      </c>
-      <c r="B458" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
-        <v>388</v>
-      </c>
-      <c r="B459" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="n">
-        <v>463</v>
-      </c>
-      <c r="B460" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="n">
-        <v>499</v>
-      </c>
-      <c r="B461" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
-        <v>334</v>
-      </c>
-      <c r="B462" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
-        <v>452</v>
-      </c>
-      <c r="B463" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="n">
-        <v>356</v>
-      </c>
-      <c r="B464" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="n">
-        <v>370</v>
-      </c>
-      <c r="B465" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
-        <v>43</v>
-      </c>
-      <c r="B466" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
-        <v>184</v>
-      </c>
-      <c r="B467" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
-        <v>168</v>
-      </c>
-      <c r="B468" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
-        <v>539</v>
-      </c>
-      <c r="B469" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="n">
-        <v>558</v>
-      </c>
-      <c r="B470" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="n">
-        <v>190</v>
-      </c>
-      <c r="B471" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>216</v>
-      </c>
-      <c r="B472" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="n">
-        <v>225</v>
-      </c>
-      <c r="B473" t="n">
         <v>23000</v>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>178</v>
-      </c>
-      <c r="B474" t="n">
         <v>23500</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>42</v>
-      </c>
-      <c r="B475" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="n">
-        <v>292</v>
-      </c>
-      <c r="B476" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="n">
-        <v>417</v>
-      </c>
-      <c r="B477" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="n">
-        <v>217</v>
-      </c>
-      <c r="B478" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="n">
-        <v>507</v>
-      </c>
-      <c r="B479" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="n">
-        <v>522</v>
-      </c>
-      <c r="B480" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="n">
-        <v>530</v>
-      </c>
-      <c r="B481" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="n">
-        <v>416</v>
-      </c>
-      <c r="B482" t="n">
         <v>24000</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="n">
-        <v>541</v>
-      </c>
-      <c r="B483" t="n">
         <v>24900</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="n">
-        <v>430</v>
-      </c>
-      <c r="B484" t="n">
         <v>24950</v>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="n">
-        <v>354</v>
-      </c>
-      <c r="B485" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="n">
-        <v>358</v>
-      </c>
-      <c r="B486" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="n">
-        <v>349</v>
-      </c>
-      <c r="B487" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="n">
-        <v>554</v>
-      </c>
-      <c r="B488" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="n">
-        <v>552</v>
-      </c>
-      <c r="B489" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="n">
-        <v>300</v>
-      </c>
-      <c r="B490" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="n">
-        <v>93</v>
-      </c>
-      <c r="B491" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="n">
-        <v>219</v>
-      </c>
-      <c r="B492" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="n">
-        <v>469</v>
-      </c>
-      <c r="B493" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="n">
-        <v>197</v>
-      </c>
-      <c r="B494" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="n">
-        <v>254</v>
-      </c>
-      <c r="B495" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="n">
-        <v>505</v>
-      </c>
-      <c r="B496" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="n">
-        <v>253</v>
-      </c>
-      <c r="B497" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="n">
-        <v>126</v>
-      </c>
-      <c r="B498" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="n">
-        <v>118</v>
-      </c>
-      <c r="B499" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="n">
-        <v>155</v>
-      </c>
-      <c r="B500" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="n">
-        <v>176</v>
-      </c>
-      <c r="B501" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="n">
-        <v>287</v>
-      </c>
-      <c r="B502" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="n">
-        <v>112</v>
-      </c>
-      <c r="B503" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="n">
-        <v>223</v>
-      </c>
-      <c r="B504" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="n">
-        <v>174</v>
-      </c>
-      <c r="B505" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="n">
-        <v>411</v>
-      </c>
-      <c r="B506" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="n">
-        <v>381</v>
-      </c>
-      <c r="B507" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="n">
-        <v>71</v>
-      </c>
-      <c r="B508" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="n">
-        <v>372</v>
-      </c>
-      <c r="B509" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="n">
-        <v>438</v>
-      </c>
-      <c r="B510" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="n">
-        <v>337</v>
-      </c>
-      <c r="B511" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="n">
-        <v>339</v>
-      </c>
-      <c r="B512" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="n">
-        <v>48</v>
-      </c>
-      <c r="B513" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="n">
-        <v>420</v>
-      </c>
-      <c r="B514" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="n">
-        <v>429</v>
-      </c>
-      <c r="B515" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="n">
-        <v>444</v>
-      </c>
-      <c r="B516" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="n">
-        <v>39</v>
-      </c>
-      <c r="B517" t="n">
         <v>25000</v>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="n">
-        <v>439</v>
-      </c>
-      <c r="B518" t="n">
         <v>25500</v>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="n">
-        <v>316</v>
-      </c>
-      <c r="B519" t="n">
         <v>25500</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="n">
-        <v>425</v>
-      </c>
-      <c r="B520" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="n">
-        <v>322</v>
-      </c>
-      <c r="B521" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="n">
-        <v>237</v>
-      </c>
-      <c r="B522" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="n">
-        <v>242</v>
-      </c>
-      <c r="B523" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="n">
-        <v>392</v>
-      </c>
-      <c r="B524" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="n">
-        <v>373</v>
-      </c>
-      <c r="B525" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="n">
-        <v>270</v>
-      </c>
-      <c r="B526" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="n">
-        <v>99</v>
-      </c>
-      <c r="B527" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="n">
-        <v>246</v>
-      </c>
-      <c r="B528" t="n">
         <v>26000</v>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="n">
-        <v>299</v>
-      </c>
-      <c r="B529" t="n">
         <v>26500</v>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="n">
-        <v>374</v>
-      </c>
-      <c r="B530" t="n">
         <v>26500</v>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="n">
-        <v>113</v>
-      </c>
-      <c r="B531" t="n">
         <v>27000</v>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="n">
-        <v>321</v>
-      </c>
-      <c r="B532" t="n">
         <v>27000</v>
       </c>
     </row>
     <row r="533">
       <c r="A533" t="n">
-        <v>382</v>
-      </c>
-      <c r="B533" t="n">
         <v>27000</v>
       </c>
     </row>
     <row r="534">
       <c r="A534" t="n">
-        <v>333</v>
-      </c>
-      <c r="B534" t="n">
         <v>27000</v>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="n">
-        <v>445</v>
-      </c>
-      <c r="B535" t="n">
         <v>27500</v>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="n">
-        <v>131</v>
-      </c>
-      <c r="B536" t="n">
         <v>27500</v>
       </c>
     </row>
     <row r="537">
       <c r="A537" t="n">
-        <v>186</v>
-      </c>
-      <c r="B537" t="n">
         <v>27500</v>
       </c>
     </row>
     <row r="538">
       <c r="A538" t="n">
-        <v>533</v>
-      </c>
-      <c r="B538" t="n">
         <v>28000</v>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="n">
-        <v>504</v>
-      </c>
-      <c r="B539" t="n">
         <v>28000</v>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="n">
-        <v>82</v>
-      </c>
-      <c r="B540" t="n">
         <v>28000</v>
       </c>
     </row>
     <row r="541">
       <c r="A541" t="n">
-        <v>17</v>
-      </c>
-      <c r="B541" t="n">
         <v>28000</v>
       </c>
     </row>
     <row r="542">
       <c r="A542" t="n">
-        <v>288</v>
-      </c>
-      <c r="B542" t="n">
         <v>29000</v>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="n">
-        <v>567</v>
-      </c>
-      <c r="B543" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="544">
       <c r="A544" t="n">
-        <v>24</v>
-      </c>
-      <c r="B544" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="545">
       <c r="A545" t="n">
-        <v>516</v>
-      </c>
-      <c r="B545" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="546">
       <c r="A546" t="n">
-        <v>301</v>
-      </c>
-      <c r="B546" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="n">
-        <v>303</v>
-      </c>
-      <c r="B547" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="n">
-        <v>233</v>
-      </c>
-      <c r="B548" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
-        <v>149</v>
-      </c>
-      <c r="B549" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="n">
-        <v>3</v>
-      </c>
-      <c r="B550" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="n">
-        <v>344</v>
-      </c>
-      <c r="B551" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="n">
-        <v>365</v>
-      </c>
-      <c r="B552" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="n">
-        <v>78</v>
-      </c>
-      <c r="B553" t="n">
         <v>30000</v>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="n">
-        <v>343</v>
-      </c>
-      <c r="B554" t="n">
         <v>32000</v>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="n">
-        <v>10</v>
-      </c>
-      <c r="B555" t="n">
         <v>32000</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="n">
-        <v>336</v>
-      </c>
-      <c r="B556" t="n">
         <v>32500</v>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="n">
-        <v>75</v>
-      </c>
-      <c r="B557" t="n">
         <v>33000</v>
       </c>
     </row>
     <row r="558">
       <c r="A558" t="n">
-        <v>19</v>
-      </c>
-      <c r="B558" t="n">
         <v>33500</v>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="n">
-        <v>141</v>
-      </c>
-      <c r="B559" t="n">
         <v>35000</v>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="n">
-        <v>314</v>
-      </c>
-      <c r="B560" t="n">
         <v>36000</v>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="n">
-        <v>76</v>
-      </c>
-      <c r="B561" t="n">
         <v>37000</v>
       </c>
     </row>
     <row r="562">
       <c r="A562" t="n">
-        <v>524</v>
-      </c>
-      <c r="B562" t="n">
         <v>37000</v>
       </c>
     </row>
     <row r="563">
       <c r="A563" t="n">
-        <v>87</v>
-      </c>
-      <c r="B563" t="n">
         <v>38000</v>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>189</v>
-      </c>
-      <c r="B564" t="n">
         <v>38000</v>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="n">
-        <v>6</v>
-      </c>
-      <c r="B565" t="n">
         <v>39000</v>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="n">
-        <v>161</v>
-      </c>
-      <c r="B566" t="n">
         <v>40000</v>
       </c>
     </row>
     <row r="567">
       <c r="A567" t="n">
-        <v>418</v>
-      </c>
-      <c r="B567" t="n">
         <v>45000</v>
       </c>
     </row>
     <row r="568">
       <c r="A568" t="n">
-        <v>240</v>
-      </c>
-      <c r="B568" t="n">
         <v>45000</v>
       </c>
     </row>
     <row r="569">
       <c r="A569" t="n">
-        <v>350</v>
-      </c>
-      <c r="B569" t="n">
         <v>45000</v>
       </c>
     </row>
     <row r="570">
       <c r="A570" t="n">
-        <v>70</v>
-      </c>
-      <c r="B570" t="n">
         <v>50000</v>
       </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>111</v>
-      </c>
-      <c r="B571" t="n">
         <v>50000</v>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>570</v>
-      </c>
-      <c r="B572" t="n">
         <v>300000</v>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>323</v>
-      </c>
-      <c r="B573" t="n">
         <v>3100000</v>
       </c>
     </row>

</xml_diff>